<commit_message>
Added 2021 First Semester Poverty Statistics
</commit_message>
<xml_diff>
--- a/Data/Poverty/Poverty.xlsx
+++ b/Data/Poverty/Poverty.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R Projects\PH-Econ-Data\Data\Poverty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90503BA0-F25C-4C4C-ABD8-3B28F670FBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F589850-2D65-4C4A-9BCE-D68514BD0152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{E463418E-18EA-45F9-8F1F-BA98B124FBDA}"/>
+    <workbookView xWindow="2040" yWindow="2670" windowWidth="17070" windowHeight="11385" activeTab="1" xr2:uid="{E463418E-18EA-45F9-8F1F-BA98B124FBDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Year" sheetId="1" r:id="rId1"/>
@@ -663,7 +663,7 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>1991</v>
+        <v>2000</v>
       </c>
       <c r="D2" s="1">
         <v>7302</v>
@@ -686,7 +686,7 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>1991</v>
+        <v>2000</v>
       </c>
       <c r="D3" s="1">
         <v>39.9</v>
@@ -709,7 +709,7 @@
         <v>15</v>
       </c>
       <c r="C4">
-        <v>1991</v>
+        <v>2000</v>
       </c>
       <c r="D4" s="1">
         <v>4780.8649999999998</v>
@@ -732,7 +732,7 @@
         <v>12</v>
       </c>
       <c r="C5">
-        <v>1991</v>
+        <v>2000</v>
       </c>
       <c r="D5" s="1">
         <v>45.3</v>
@@ -755,7 +755,7 @@
         <v>14</v>
       </c>
       <c r="C6">
-        <v>1991</v>
+        <v>2000</v>
       </c>
       <c r="D6" s="1">
         <v>28119.758000000002</v>
@@ -778,7 +778,7 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <v>1991</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -789,7 +789,7 @@
         <v>12</v>
       </c>
       <c r="C8">
-        <v>1991</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -800,7 +800,7 @@
         <v>15</v>
       </c>
       <c r="C9">
-        <v>1991</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -811,7 +811,7 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>1991</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -822,7 +822,7 @@
         <v>14</v>
       </c>
       <c r="C11">
-        <v>1991</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -833,7 +833,7 @@
         <v>12</v>
       </c>
       <c r="C12">
-        <v>1991</v>
+        <v>2000</v>
       </c>
       <c r="D12" s="1">
         <v>32.700000000000003</v>
@@ -856,7 +856,7 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>1991</v>
+        <v>2000</v>
       </c>
       <c r="D13" s="1">
         <v>13</v>
@@ -879,7 +879,7 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>1991</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -890,7 +890,7 @@
         <v>11</v>
       </c>
       <c r="C15">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="G15" s="1">
         <v>11458.499451251928</v>
@@ -910,7 +910,7 @@
         <v>12</v>
       </c>
       <c r="C16">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="G16" s="1">
         <v>27.453544103072574</v>
@@ -930,7 +930,7 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="G17" s="1">
         <v>4146.6630985908496</v>
@@ -950,7 +950,7 @@
         <v>12</v>
       </c>
       <c r="C18">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="G18" s="1">
         <v>33.023020205590861</v>
@@ -970,7 +970,7 @@
         <v>14</v>
       </c>
       <c r="C19">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="G19" s="1">
         <v>25472.782191081998</v>
@@ -990,7 +990,7 @@
         <v>11</v>
       </c>
       <c r="C20">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="G20" s="1">
         <v>7707.2214177156284</v>
@@ -1010,7 +1010,7 @@
         <v>12</v>
       </c>
       <c r="C21">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="G21" s="1">
         <v>12.273644682193549</v>
@@ -1030,7 +1030,7 @@
         <v>15</v>
       </c>
       <c r="C22">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="G22" s="1">
         <v>1849.87649799728</v>
@@ -1050,7 +1050,7 @@
         <v>12</v>
       </c>
       <c r="C23">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="G23" s="1">
         <v>15.816183342524578</v>
@@ -1070,7 +1070,7 @@
         <v>14</v>
       </c>
       <c r="C24">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="G24" s="1">
         <v>12200.0407857952</v>
@@ -1090,7 +1090,7 @@
         <v>12</v>
       </c>
       <c r="C25">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="G25" s="1">
         <v>29.1</v>
@@ -1110,7 +1110,7 @@
         <v>12</v>
       </c>
       <c r="C26">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="G26" s="1">
         <v>7.9992048923048227</v>
@@ -1130,7 +1130,7 @@
         <v>12</v>
       </c>
       <c r="C27">
-        <v>2000</v>
+        <v>2006</v>
       </c>
       <c r="G27" s="1">
         <v>3.4384822643916801</v>
@@ -1150,7 +1150,7 @@
         <v>11</v>
       </c>
       <c r="C28">
-        <v>2006</v>
+        <v>2015</v>
       </c>
       <c r="I28" s="1">
         <v>13357.419556264384</v>
@@ -1173,7 +1173,7 @@
         <v>12</v>
       </c>
       <c r="C29">
-        <v>2006</v>
+        <v>2015</v>
       </c>
       <c r="I29" s="1">
         <v>21.00836</v>
@@ -1196,7 +1196,7 @@
         <v>15</v>
       </c>
       <c r="C30">
-        <v>2006</v>
+        <v>2015</v>
       </c>
       <c r="I30" s="1">
         <v>3809.2829999999999</v>
@@ -1219,7 +1219,7 @@
         <v>12</v>
       </c>
       <c r="C31">
-        <v>2006</v>
+        <v>2015</v>
       </c>
       <c r="I31" s="1">
         <v>26.561420000000002</v>
@@ -1242,7 +1242,7 @@
         <v>14</v>
       </c>
       <c r="C32">
-        <v>2006</v>
+        <v>2015</v>
       </c>
       <c r="I32" s="1">
         <v>22643.980199999998</v>
@@ -1265,7 +1265,7 @@
         <v>11</v>
       </c>
       <c r="C33">
-        <v>2006</v>
+        <v>2015</v>
       </c>
       <c r="I33" s="1">
         <v>9308.0753713642098</v>
@@ -1288,7 +1288,7 @@
         <v>12</v>
       </c>
       <c r="C34">
-        <v>2006</v>
+        <v>2015</v>
       </c>
       <c r="I34" s="1">
         <v>8.8066899999999997</v>
@@ -1311,7 +1311,7 @@
         <v>15</v>
       </c>
       <c r="C35">
-        <v>2006</v>
+        <v>2015</v>
       </c>
       <c r="I35" s="1">
         <v>1596.85</v>
@@ -1334,7 +1334,7 @@
         <v>12</v>
       </c>
       <c r="C36">
-        <v>2006</v>
+        <v>2015</v>
       </c>
       <c r="I36" s="1">
         <v>12.003679999999999</v>
@@ -1357,7 +1357,7 @@
         <v>14</v>
       </c>
       <c r="C37">
-        <v>2006</v>
+        <v>2015</v>
       </c>
       <c r="I37" s="1">
         <v>10233.303750000003</v>
@@ -1380,7 +1380,7 @@
         <v>12</v>
       </c>
       <c r="C38">
-        <v>2006</v>
+        <v>2015</v>
       </c>
       <c r="I38" s="1">
         <v>27.456799999999998</v>
@@ -1403,7 +1403,7 @@
         <v>12</v>
       </c>
       <c r="C39">
-        <v>2006</v>
+        <v>2015</v>
       </c>
       <c r="I39" s="1">
         <v>5.7682200000000003</v>
@@ -1426,7 +1426,7 @@
         <v>12</v>
       </c>
       <c r="C40">
-        <v>2006</v>
+        <v>2015</v>
       </c>
       <c r="I40" s="1">
         <v>2.2499600000000002</v>
@@ -1449,7 +1449,7 @@
         <v>11</v>
       </c>
       <c r="C41">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="L41" s="1">
         <v>22746.746510438112</v>
@@ -1466,7 +1466,7 @@
         <v>12</v>
       </c>
       <c r="C42">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="L42" s="1">
         <v>18.012219559473095</v>
@@ -1483,7 +1483,7 @@
         <v>15</v>
       </c>
       <c r="C43">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="L43" s="1">
         <v>4138.4205548000027</v>
@@ -1500,7 +1500,7 @@
         <v>12</v>
       </c>
       <c r="C44">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="L44" s="1">
         <v>23.482021781699945</v>
@@ -1517,7 +1517,7 @@
         <v>14</v>
       </c>
       <c r="C45">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="L45" s="1">
         <v>23677.714031402589</v>
@@ -1534,7 +1534,7 @@
         <v>11</v>
       </c>
       <c r="C46">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="L46" s="1">
         <v>15887.438663852547</v>
@@ -1551,7 +1551,7 @@
         <v>12</v>
       </c>
       <c r="C47">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="L47" s="1">
         <v>6.484108714076962</v>
@@ -1568,7 +1568,7 @@
         <v>15</v>
       </c>
       <c r="C48">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="L48" s="1">
         <v>1489.7646952000005</v>
@@ -1585,7 +1585,7 @@
         <v>12</v>
       </c>
       <c r="C49">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="L49" s="1">
         <v>9.1394857594723025</v>
@@ -1602,7 +1602,7 @@
         <v>14</v>
       </c>
       <c r="C50">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="L50" s="1">
         <v>9215.6515405120845</v>
@@ -1619,7 +1619,7 @@
         <v>12</v>
       </c>
       <c r="C51">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="L51" s="1">
         <v>25.135367091627455</v>
@@ -1636,7 +1636,7 @@
         <v>12</v>
       </c>
       <c r="C52">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="L52" s="1">
         <v>4.5274375076234836</v>
@@ -1653,7 +1653,7 @@
         <v>12</v>
       </c>
       <c r="C53">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="L53" s="1">
         <v>1.6637704068693198</v>
@@ -1670,9 +1670,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5646DEA-C981-45F2-BF15-5300648A4A42}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1720,8 +1720,8 @@
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
+      <c r="C2">
+        <v>2015</v>
       </c>
       <c r="D2" s="1">
         <v>6702.9085889219659</v>
@@ -1743,8 +1743,8 @@
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
+      <c r="C3">
+        <v>2015</v>
       </c>
       <c r="D3" s="1">
         <v>23.378029999999999</v>
@@ -1766,8 +1766,8 @@
       <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
+      <c r="C4">
+        <v>2015</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1777,8 +1777,8 @@
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
+      <c r="C5">
+        <v>2015</v>
       </c>
       <c r="D5" s="1">
         <v>28.788130000000002</v>
@@ -1800,8 +1800,8 @@
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
+      <c r="C6">
+        <v>2015</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1811,8 +1811,8 @@
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
-        <v>13</v>
+      <c r="C7">
+        <v>2015</v>
       </c>
       <c r="D7" s="1">
         <v>4673.1672249300664</v>
@@ -1834,8 +1834,8 @@
       <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
-        <v>13</v>
+      <c r="C8">
+        <v>2015</v>
       </c>
       <c r="D8" s="1">
         <v>10.84394</v>
@@ -1857,8 +1857,8 @@
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
-        <v>13</v>
+      <c r="C9">
+        <v>2015</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1868,8 +1868,8 @@
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
-        <v>13</v>
+      <c r="C10">
+        <v>2015</v>
       </c>
       <c r="D10" s="1">
         <v>14.23226</v>
@@ -1891,8 +1891,8 @@
       <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C11" t="s">
-        <v>13</v>
+      <c r="C11">
+        <v>2015</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1902,8 +1902,8 @@
       <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
-        <v>13</v>
+      <c r="C12">
+        <v>2015</v>
       </c>
       <c r="D12" s="1">
         <v>30.070530000000002</v>
@@ -1925,8 +1925,8 @@
       <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
-        <v>13</v>
+      <c r="C13">
+        <v>2015</v>
       </c>
       <c r="D13" s="1">
         <v>7.0298999999999996</v>
@@ -1948,8 +1948,8 @@
       <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
-        <v>13</v>
+      <c r="C14">
+        <v>2015</v>
       </c>
       <c r="D14" s="1">
         <v>2.9904600000000001</v>
@@ -1971,8 +1971,8 @@
       <c r="B15" t="s">
         <v>11</v>
       </c>
-      <c r="C15" t="s">
-        <v>21</v>
+      <c r="C15">
+        <v>2018</v>
       </c>
       <c r="G15" s="1">
         <v>11343.554197223561</v>
@@ -1988,8 +1988,8 @@
       <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="C16" t="s">
-        <v>21</v>
+      <c r="C16">
+        <v>2018</v>
       </c>
       <c r="G16" s="1">
         <v>22.20016</v>
@@ -1998,26 +1998,26 @@
         <v>16.11421</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
       </c>
-      <c r="C18" t="s">
-        <v>21</v>
+      <c r="C18">
+        <v>2018</v>
       </c>
       <c r="G18" s="1">
         <v>27.628910000000001</v>
@@ -2026,26 +2026,26 @@
         <v>20.999960000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>14</v>
       </c>
-      <c r="C19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
-      <c r="C20" t="s">
-        <v>21</v>
+      <c r="C20">
+        <v>2018</v>
       </c>
       <c r="G20" s="1">
         <v>7920.1942015328677</v>
@@ -2054,15 +2054,15 @@
         <v>8803.8365655750877</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>
       </c>
-      <c r="C21" t="s">
-        <v>21</v>
+      <c r="C21">
+        <v>2018</v>
       </c>
       <c r="G21" s="1">
         <v>9.8804199999999991</v>
@@ -2071,26 +2071,26 @@
         <v>6.1650900000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
       <c r="B22" t="s">
         <v>15</v>
       </c>
-      <c r="C22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="B23" t="s">
         <v>12</v>
       </c>
-      <c r="C23" t="s">
-        <v>21</v>
+      <c r="C23">
+        <v>2018</v>
       </c>
       <c r="G23" s="1">
         <v>13.011139999999999</v>
@@ -2099,26 +2099,26 @@
         <v>8.4680400000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="B24" t="s">
         <v>14</v>
       </c>
-      <c r="C24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
       <c r="B25" t="s">
         <v>12</v>
       </c>
-      <c r="C25" t="s">
-        <v>21</v>
+      <c r="C25">
+        <v>2018</v>
       </c>
       <c r="G25" s="1">
         <v>29.51285</v>
@@ -2127,15 +2127,15 @@
         <v>26.949159999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
       <c r="B26" t="s">
         <v>12</v>
       </c>
-      <c r="C26" t="s">
-        <v>21</v>
+      <c r="C26">
+        <v>2018</v>
       </c>
       <c r="G26" s="1">
         <v>6.5518999999999998</v>
@@ -2144,21 +2144,242 @@
         <v>4.3426499999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
       <c r="B27" t="s">
         <v>12</v>
       </c>
-      <c r="C27" t="s">
-        <v>21</v>
+      <c r="C27">
+        <v>2018</v>
       </c>
       <c r="G27" s="1">
         <v>2.7593099999999997</v>
       </c>
       <c r="H27" s="1">
         <v>1.7868599999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28">
+        <v>2021</v>
+      </c>
+      <c r="H28" s="1">
+        <v>12637.918553006057</v>
+      </c>
+      <c r="I28" s="1">
+        <v>14498.078114544631</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <v>2021</v>
+      </c>
+      <c r="H29" s="1">
+        <v>16.187536428016173</v>
+      </c>
+      <c r="I29" s="1">
+        <v>17.955553145557833</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30">
+        <v>2021</v>
+      </c>
+      <c r="H30" s="1">
+        <v>4039.4099904000514</v>
+      </c>
+      <c r="I30" s="1">
+        <v>4739.8110360999972</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31">
+        <v>2021</v>
+      </c>
+      <c r="H31" s="1">
+        <v>21.050909176398534</v>
+      </c>
+      <c r="I31" s="1">
+        <v>23.717926630826302</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32">
+        <v>2021</v>
+      </c>
+      <c r="H32" s="1">
+        <v>22262.427214906216</v>
+      </c>
+      <c r="I32" s="1">
+        <v>26136.836813200051</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <v>2021</v>
+      </c>
+      <c r="H33" s="1">
+        <v>8848.5788319105577</v>
+      </c>
+      <c r="I33" s="1">
+        <v>10071.257720130052</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34">
+        <v>2021</v>
+      </c>
+      <c r="H34" s="1">
+        <v>6.2078326218868618</v>
+      </c>
+      <c r="I34" s="1">
+        <v>7.0792336675070695</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35">
+        <v>2021</v>
+      </c>
+      <c r="H35" s="1">
+        <v>1549.0918721999913</v>
+      </c>
+      <c r="I35" s="1">
+        <v>1868.7383002000088</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36">
+        <v>2021</v>
+      </c>
+      <c r="H36" s="1">
+        <v>8.5392721451641069</v>
+      </c>
+      <c r="I36" s="1">
+        <v>9.9320081650149685</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37">
+        <v>2021</v>
+      </c>
+      <c r="H37" s="1">
+        <v>9030.7227591447827</v>
+      </c>
+      <c r="I37" s="1">
+        <v>10944.939693799992</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>2021</v>
+      </c>
+      <c r="H38" s="1">
+        <v>26.97636346869961</v>
+      </c>
+      <c r="I38" s="1">
+        <v>27.037492166175564</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39">
+        <v>2021</v>
+      </c>
+      <c r="H39" s="1">
+        <v>4.3668086634497962</v>
+      </c>
+      <c r="I39" s="1">
+        <v>4.8547312751236902</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>2021</v>
+      </c>
+      <c r="H40" s="1">
+        <v>1.7974468063177669</v>
+      </c>
+      <c r="I40" s="1">
+        <v>1.9483855219994111</v>
       </c>
     </row>
   </sheetData>
@@ -3694,7 +3915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4BEF0A-7E2D-4824-9721-1722416055A8}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added 2021 Full Year Poverty Statistics
</commit_message>
<xml_diff>
--- a/Data/Poverty/Poverty.xlsx
+++ b/Data/Poverty/Poverty.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R Projects\PH-Econ-Data\Data\Poverty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F589850-2D65-4C4A-9BCE-D68514BD0152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3B9911-5E88-4BB5-A408-F8677D19D872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="2670" windowWidth="17070" windowHeight="11385" activeTab="1" xr2:uid="{E463418E-18EA-45F9-8F1F-BA98B124FBDA}"/>
+    <workbookView xWindow="9675" yWindow="4245" windowWidth="18570" windowHeight="10815" xr2:uid="{E463418E-18EA-45F9-8F1F-BA98B124FBDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Year" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="59">
   <si>
     <t>Indicator</t>
   </si>
@@ -186,9 +186,6 @@
     <t>Self-Employed and Unpaid Family Workers</t>
   </si>
   <si>
-    <t>2015-2018 (Poverty Statistics)</t>
-  </si>
-  <si>
     <t>2006-2015 (Poverty Statistics)</t>
   </si>
   <si>
@@ -211,6 +208,12 @@
   </si>
   <si>
     <t>1994</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>2015-2021 (Poverty Statistics)</t>
   </si>
 </sst>
 </file>
@@ -599,11 +602,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23EFC0EE-14C2-43E0-ACDC-93DE3602A4AE}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +617,7 @@
     <col min="4" max="15" width="10.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -625,19 +628,19 @@
         <v>10</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I1" s="4">
         <v>2006</v>
@@ -654,8 +657,11 @@
       <c r="M1" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -678,7 +684,7 @@
         <v>13823</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -701,7 +707,7 @@
         <v>33.700000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -724,7 +730,7 @@
         <v>5139.5649999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -747,7 +753,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -770,7 +776,7 @@
         <v>30850.191999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -781,7 +787,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -792,7 +798,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -803,7 +809,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -814,7 +820,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -825,7 +831,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -848,7 +854,7 @@
         <v>31.78</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -871,7 +877,7 @@
         <v>10.71</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -882,7 +888,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -902,7 +908,7 @@
         <v>15057.197726169672</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1257,7 +1263,7 @@
         <v>21927.009399999999</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -1280,7 +1286,7 @@
         <v>15189</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -1303,7 +1309,7 @@
         <v>5.7348299999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -1326,7 +1332,7 @@
         <v>1303.549</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -1349,7 +1355,7 @@
         <v>8.0991900000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -1372,7 +1378,7 @@
         <v>8225.7214999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -1395,7 +1401,7 @@
         <v>24.6</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1418,7 +1424,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -1441,7 +1447,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -1457,8 +1463,11 @@
       <c r="M41" s="1">
         <v>25813.497824622897</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41" s="1">
+        <v>28871.319939449077</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1</v>
       </c>
@@ -1474,8 +1483,11 @@
       <c r="M42" s="1">
         <v>12.141213642319308</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N42" s="1">
+        <v>13.245432215865016</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -1491,8 +1503,11 @@
       <c r="M43" s="1">
         <v>3004.6072561000165</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N43" s="1">
+        <v>3496.4584590999966</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -1508,8 +1523,11 @@
       <c r="M44" s="1">
         <v>16.708595917138165</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N44" s="1">
+        <v>18.142008108986257</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>18</v>
       </c>
@@ -1525,8 +1543,11 @@
       <c r="M45" s="1">
         <v>17670.205910017012</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N45" s="1">
+        <v>19992.249267000123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -1542,8 +1563,11 @@
       <c r="M46" s="1">
         <v>18126.108777562113</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N46" s="1">
+        <v>20110.526033729573</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -1559,8 +1583,11 @@
       <c r="M47" s="1">
         <v>3.3924762787208991</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N47" s="1">
+        <v>3.9374862805873128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -1576,8 +1603,11 @@
       <c r="M48" s="1">
         <v>839.54200490000107</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N48" s="1">
+        <v>1039.3966002000031</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -1593,8 +1623,11 @@
       <c r="M49" s="1">
         <v>5.2390968558636484</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N49" s="1">
+        <v>5.9396263055465885</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -1605,13 +1638,16 @@
         <v>2018</v>
       </c>
       <c r="L50" s="1">
-        <v>9215.6515405120845</v>
+        <v>9215.6515405120863</v>
       </c>
       <c r="M50" s="1">
         <v>5540.6163800201412</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N50" s="1">
+        <v>6545.3884123500029</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -1627,8 +1663,11 @@
       <c r="M51" s="1">
         <v>21.731107023541483</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N51" s="1">
+        <v>22.554584635075997</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -1644,8 +1683,11 @@
       <c r="M52" s="1">
         <v>2.6384201305692279</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N52" s="1">
+        <v>2.9874522194088966</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -1660,6 +1702,9 @@
       </c>
       <c r="M53" s="1">
         <v>0.87039642515473603</v>
+      </c>
+      <c r="N53" s="1">
+        <v>1.0135076257860098</v>
       </c>
     </row>
   </sheetData>
@@ -1672,11 +1717,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5646DEA-C981-45F2-BF15-5300648A4A42}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1687,7 +1732,7 @@
     <col min="4" max="10" width="10.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1712,8 +1757,11 @@
       <c r="H1" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1736,7 +1784,7 @@
         <v>10968.529156205745</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1759,7 +1807,7 @@
         <v>21.065909999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1770,7 +1818,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1793,7 +1841,7 @@
         <v>26.339269999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1804,7 +1852,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1827,7 +1875,7 @@
         <v>7638.0556724844619</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1850,7 +1898,7 @@
         <v>9.1606400000000008</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1861,7 +1909,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1884,7 +1932,7 @@
         <v>12.06002</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1895,7 +1943,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1918,7 +1966,7 @@
         <v>28.981400000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1941,7 +1989,7 @@
         <v>6.1052</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1964,7 +2012,7 @@
         <v>2.5419800000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1981,7 +2029,7 @@
         <v>12576.652532652335</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -3916,7 +3964,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3961,7 +4009,7 @@
         <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3977,7 +4025,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3985,7 +4033,7 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3993,7 +4041,7 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -4001,7 +4049,7 @@
         <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added 2021 Preliminary Basic Sector Poverty Statistics
</commit_message>
<xml_diff>
--- a/Data/Poverty/Poverty.xlsx
+++ b/Data/Poverty/Poverty.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R Projects\PH-Econ-Data\Data\Poverty\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R-Projects\PH-Econ-Data\Data\Poverty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3B9911-5E88-4BB5-A408-F8677D19D872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D56B646-874C-41D8-8DE9-F59F3606228B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9675" yWindow="4245" windowWidth="18570" windowHeight="10815" xr2:uid="{E463418E-18EA-45F9-8F1F-BA98B124FBDA}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="2" xr2:uid="{E463418E-18EA-45F9-8F1F-BA98B124FBDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Year" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="82">
   <si>
     <t>Indicator</t>
   </si>
@@ -214,6 +214,107 @@
   </si>
   <si>
     <t>2015-2021 (Poverty Statistics)</t>
+  </si>
+  <si>
+    <t>Operational Definition</t>
+  </si>
+  <si>
+    <t>Urban Poor</t>
+  </si>
+  <si>
+    <t>Rural Poor</t>
+  </si>
+  <si>
+    <t>Migant and Formal Sector Workers</t>
+  </si>
+  <si>
+    <t>Fisherfolks</t>
+  </si>
+  <si>
+    <t>Self-employed and Unpaid Family Workers</t>
+  </si>
+  <si>
+    <t>Persons with Disability</t>
+  </si>
+  <si>
+    <t>Individuals below 18 years old</t>
+  </si>
+  <si>
+    <t>An individual whose declared sex is female</t>
+  </si>
+  <si>
+    <t>Individuals 15 to 30 years old</t>
+  </si>
+  <si>
+    <t>Individuals 60 years old and above</t>
+  </si>
+  <si>
+    <t>An individual residing in an urban area who belongs to a poor family or whose per capita income falls below the official  poverty threshold. Urban classification used in the estimates for 2015 and 2018 is based on the 2015 Census of Population</t>
+  </si>
+  <si>
+    <t>An individual residing in a rural area who belongs to a family categorized as poor or with per capita income falling below the official poverty threshold</t>
+  </si>
+  <si>
+    <t>Migrant workers are individuals who are overseas contract workers (OCWs).
+or
+Formal sector workers are employed persons working for private establishments and government organizations and corporations</t>
+  </si>
+  <si>
+    <t>Employed individuals 15 years old and over whose primary occupation is farming and plant growing or animal production.
+In the 2012 Philippine Standard Occupational Classification (PSOC), which was also adopted in the January 2019 LFS, the following occupations were considered:
+a) Under Major Occupation 6 – Skilled Agricultural, Forestry and Fishery Works
+   i) Market gardeners and crop growers;
+   ii) Animal producers; iii) Mixed crop and animal producers;
+   iii) Subsistence crop farmers;
+   iv) Subsistence livestock farmers; and
+   v) Subsistence mixed crop and livestock farmers.
+(Note: These are minor occupation groups.)
+b) Under Major Occupation 9 – Elementary Occupations
+   i) Crop farm laborers;
+   ii) Livestock farm laborers;
+   iii) Mixed crop and livestock farm laborers; and
+   iv) Garden and horticultural laborers.
+(Note: These are unit occupation groups.)</t>
+  </si>
+  <si>
+    <t>Employed individuals 15 years old and over who are either self-employed or worked without pay on family-owned business.</t>
+  </si>
+  <si>
+    <t>Persons with disability are those who experienced a lot of difficulty or who cannot do at all any of the following:
+   a) Seeing even if wearing eye-glasses;
+   b) Hearing even if using hearing aid;
+   c) Walking or climbing steps;
+   d) Remembering or concentrating;
+   e) Self-care; and
+   f) Communicating.
+The Washington Group on Disability Statistics recommended this cut-off for disability.</t>
+  </si>
+  <si>
+    <t>Employed individuals 15 years old and over whose primary occupation is fishing.
+In the 2012 Philippine Standard Occupational Classification (PSOC), which the January 2019 LFS adopted, the following occupations were considered:
+a) Under Major Occupation 6 – Skilled Agricultural, Forestry and Fishery Works
+   i) Fishery workers; and
+   ii) Subsistence fishers
+(Note: These are minor occupation groups.)
+b) Under Major Occupation 9 – Elementary Occupations
+   i) Fishery and aquaculture laborers
+(Note: This is a unit occupation group.)</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Poverty is a characteristic of the family. Thus, if a family is classified as poor, then all members of the family will be counted as poor. In other words, a family cannot have poor and non-poor members. Either all members are poor or all members are non-poor.</t>
+  </si>
+  <si>
+    <t>Total family income divided by the family size is used to generate annual per capita income, which is then compared with the annual per capita poverty threshold to determine the poverty status of the family and not the individual income.</t>
+  </si>
+  <si>
+    <t>Basic sectors are not mutually exclusive, i.e., there are overlaps among the sectors, which means an individual can belong to two or more sectors (e.g., women and children, women and senior citizens, youth and individuals residing in urban areas, etc.).</t>
+  </si>
+  <si>
+    <t>For the estimation of poverty and subsistence incidence, the FIES was utilized for classifying families as poor or non-poor and food poor or non-food poor, respectively, while the LFS was used to classify family members into basic sectors with disaggregation at the national and regional levels. Both FIES and LFS follow the Integrated Survey of Households (ISH) sampling scheme where the sample families in the FIES are generally the same sample families in the LFS.
+The food and poverty thresholds used to identify, whether the families are poor or not, were taken from the Full Year Official Poverty Statistics released by PSA.</t>
   </si>
 </sst>
 </file>
@@ -275,16 +376,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -602,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23EFC0EE-14C2-43E0-ACDC-93DE3602A4AE}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E38" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="N54" sqref="N54"/>
@@ -617,47 +738,47 @@
     <col min="4" max="15" width="10.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="4">
+      <c r="I1" s="2">
         <v>2006</v>
       </c>
-      <c r="J1" s="4">
+      <c r="J1" s="2">
         <v>2009</v>
       </c>
-      <c r="K1" s="4">
+      <c r="K1" s="2">
         <v>2012</v>
       </c>
-      <c r="L1" s="4">
+      <c r="L1" s="2">
         <v>2015</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="2" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1732,32 +1853,32 @@
     <col min="4" max="10" width="10.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="2">
         <v>2006</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="2">
         <v>2009</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="2">
         <v>2012</v>
       </c>
-      <c r="G1" s="4">
+      <c r="G1" s="2">
         <v>2015</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2440,11 +2561,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37D2146-B4B8-46DC-9C0C-C94E3AE61587}">
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I82" sqref="I82"/>
+      <selection pane="bottomRight" activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2453,40 +2574,42 @@
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="9" width="10.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="1"/>
+    <col min="5" max="10" width="10.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="2">
         <v>2006</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="2">
         <v>2009</v>
       </c>
-      <c r="G1" s="4">
+      <c r="G1" s="2">
         <v>2012</v>
       </c>
-      <c r="H1" s="4">
+      <c r="H1" s="2">
         <v>2015</v>
       </c>
-      <c r="I1" s="4">
+      <c r="I1" s="2">
         <v>2018</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -2512,7 +2635,7 @@
         <v>22.499300000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -2526,7 +2649,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -2540,7 +2663,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -2554,7 +2677,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -2580,7 +2703,7 @@
         <v>31.4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -2594,7 +2717,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -2608,7 +2731,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -2622,7 +2745,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -2648,7 +2771,7 @@
         <v>19.381900000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -2662,7 +2785,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -2676,7 +2799,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -2690,7 +2813,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -2716,7 +2839,7 @@
         <v>13.1503</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2730,7 +2853,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -3004,7 +3127,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -3018,7 +3141,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -3044,7 +3167,7 @@
         <v>33.978400000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -3058,7 +3181,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -3072,7 +3195,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -3086,7 +3209,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -3112,7 +3235,7 @@
         <v>25.0136</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -3126,7 +3249,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -3140,7 +3263,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -3154,7 +3277,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -3173,8 +3296,11 @@
       <c r="I42" s="1">
         <v>16.558168759736759</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" s="1">
+        <v>18.403915621292001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -3193,8 +3319,11 @@
       <c r="I43" s="1">
         <v>8655.6983603001045</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" s="1">
+        <v>9985.7989651001499</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>37</v>
       </c>
@@ -3213,8 +3342,11 @@
       <c r="I44" s="1">
         <v>5.2173332811708839</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" s="1">
+        <v>6.0873192334868804</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -3233,8 +3365,11 @@
       <c r="I45" s="1">
         <v>2727.3343919999984</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="1">
+        <v>3302.9246250000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>35</v>
       </c>
@@ -3253,8 +3388,11 @@
       <c r="I46" s="1">
         <v>23.886119310623695</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" s="1">
+        <v>26.401041287602698</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -3273,8 +3411,11 @@
       <c r="I47" s="1">
         <v>9340.7257055000591</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" s="1">
+        <v>10463.423518600201</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -3293,8 +3434,11 @@
       <c r="I48" s="1">
         <v>8.0665061046746622</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" s="1">
+        <v>9.4169870468526504</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>38</v>
       </c>
@@ -3313,8 +3457,11 @@
       <c r="I49" s="1">
         <v>3154.4270521999806</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" s="1">
+        <v>3732.1983881999799</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>35</v>
       </c>
@@ -3333,8 +3480,11 @@
       <c r="I50" s="1">
         <v>14.746623506720944</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" s="1">
+        <v>16.581417347140299</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -3353,8 +3503,11 @@
       <c r="I51" s="1">
         <v>4481.4151366000133</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" s="1">
+        <v>5124.1318035000204</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -3373,8 +3526,11 @@
       <c r="I52" s="1">
         <v>4.4359836931803081</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52" s="1">
+        <v>5.1067968737089702</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>38</v>
       </c>
@@ -3393,8 +3549,11 @@
       <c r="I53" s="1">
         <v>1348.0702520999978</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53" s="1">
+        <v>1578.1461697</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>35</v>
       </c>
@@ -3413,8 +3572,11 @@
       <c r="I54" s="1">
         <v>9.1251097652432041</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54" s="1">
+        <v>10.259814778598299</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -3433,8 +3595,11 @@
       <c r="I55" s="1">
         <v>829.2054251000003</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J55" s="1">
+        <v>1019.2600154</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>37</v>
       </c>
@@ -3453,8 +3618,11 @@
       <c r="I56" s="1">
         <v>2.2269353727442662</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J56" s="1">
+        <v>2.8226748703290498</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>38</v>
       </c>
@@ -3473,8 +3641,11 @@
       <c r="I57" s="1">
         <v>202.36325260000004</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J57" s="1">
+        <v>280.41828179999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>35</v>
       </c>
@@ -3493,8 +3664,11 @@
       <c r="I58" s="1">
         <v>9.3043550793306657</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J58" s="1">
+        <v>11.6471560559305</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>36</v>
       </c>
@@ -3513,8 +3687,11 @@
       <c r="I59" s="1">
         <v>5037.7924518000054</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J59" s="1">
+        <v>6580.9748668000802</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>37</v>
       </c>
@@ -3533,8 +3710,11 @@
       <c r="I60" s="1">
         <v>2.6198681930499839</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J60" s="1">
+        <v>3.3166836588497599</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>38</v>
       </c>
@@ -3553,8 +3733,11 @@
       <c r="I61" s="1">
         <v>1418.5133838000079</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J61" s="1">
+        <v>1874.0207218999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>35</v>
       </c>
@@ -3573,8 +3756,11 @@
       <c r="I62" s="1">
         <v>24.455686151937428</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J62" s="1">
+        <v>25.6816699304655</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>36</v>
       </c>
@@ -3593,8 +3779,11 @@
       <c r="I63" s="1">
         <v>12644.425654099812</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J63" s="1">
+        <v>13673.1648926</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>37</v>
       </c>
@@ -3613,8 +3802,11 @@
       <c r="I64" s="1">
         <v>8.0023639672063833</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J64" s="1">
+        <v>9.0141457279387005</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>38</v>
       </c>
@@ -3633,8 +3825,11 @@
       <c r="I65" s="1">
         <v>4137.4956978000091</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J65" s="1">
+        <v>4799.2167657999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>35</v>
       </c>
@@ -3653,8 +3848,11 @@
       <c r="I66" s="1">
         <v>8.769059525062751</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J66" s="1">
+        <v>10.195046696992399</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>36</v>
       </c>
@@ -3673,8 +3871,11 @@
       <c r="I67" s="1">
         <v>2385.8834701999958</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J67" s="1">
+        <v>2803.5885965999901</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>37</v>
       </c>
@@ -3693,8 +3894,11 @@
       <c r="I68" s="1">
         <v>2.0919469209704937</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J68" s="1">
+        <v>2.6286208974973002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>38</v>
       </c>
@@ -3713,8 +3917,11 @@
       <c r="I69" s="1">
         <v>569.17638259999853</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J69" s="1">
+        <v>722.8580498</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>35</v>
       </c>
@@ -3733,8 +3940,11 @@
       <c r="I70" s="1">
         <v>31.596468444757914</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J70" s="1">
+        <v>30.0161704040068</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>36</v>
       </c>
@@ -3753,8 +3963,11 @@
       <c r="I71" s="1">
         <v>2381.6678780000107</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J71" s="1">
+        <v>2371.4588973</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>37</v>
       </c>
@@ -3773,8 +3986,11 @@
       <c r="I72" s="1">
         <v>11.484312013255666</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J72" s="1">
+        <v>10.6875658236438</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>38</v>
       </c>
@@ -3793,8 +4009,11 @@
       <c r="I73" s="1">
         <v>865.66057440000145</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J73" s="1">
+        <v>844.38230199999805</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>35</v>
       </c>
@@ -3813,8 +4032,11 @@
       <c r="I74" s="1">
         <v>26.199814315355429</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J74" s="1">
+        <v>30.636770131799999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>36</v>
       </c>
@@ -3833,8 +4055,11 @@
       <c r="I75" s="1">
         <v>287.07144290000036</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J75" s="1">
+        <v>348.2808766</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>37</v>
       </c>
@@ -3853,8 +4078,11 @@
       <c r="I76" s="1">
         <v>8.2644355909764045</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J76" s="1">
+        <v>10.772162205654899</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>38</v>
       </c>
@@ -3873,8 +4101,11 @@
       <c r="I77" s="1">
         <v>90.553445200000013</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J77" s="1">
+        <v>122.45866909999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>35</v>
       </c>
@@ -3893,8 +4124,11 @@
       <c r="I78" s="1">
         <v>17.986587966677497</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J78" s="1">
+        <v>18.671349623259001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>36</v>
       </c>
@@ -3913,8 +4147,11 @@
       <c r="I79" s="1">
         <v>2251.2354339000017</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J79" s="1">
+        <v>2517.8806740999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>37</v>
       </c>
@@ -3933,8 +4170,11 @@
       <c r="I80" s="1">
         <v>6.245019896879028</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J80" s="1">
+        <v>6.3678341440460402</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>38</v>
       </c>
@@ -3952,6 +4192,9 @@
       </c>
       <c r="I81" s="1">
         <v>781.63852440000051</v>
+      </c>
+      <c r="J81" s="1">
+        <v>858.71920619999798</v>
       </c>
     </row>
   </sheetData>
@@ -3961,105 +4204,222 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4BEF0A-7E2D-4824-9721-1722416055A8}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="36.5703125" customWidth="1"/>
+    <col min="1" max="1" width="36.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="8"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B8" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+    <row r="15" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="390" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>75</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added 2021 Poverty Data
</commit_message>
<xml_diff>
--- a/Data/Poverty/Poverty.xlsx
+++ b/Data/Poverty/Poverty.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R-Projects\PH-Econ-Data\Data\Poverty\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Poverty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D56B646-874C-41D8-8DE9-F59F3606228B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3261155-FD70-48E6-8484-2EAB479F65D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="2" xr2:uid="{E463418E-18EA-45F9-8F1F-BA98B124FBDA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E463418E-18EA-45F9-8F1F-BA98B124FBDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Year" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="83">
   <si>
     <t>Indicator</t>
   </si>
@@ -315,6 +315,9 @@
   <si>
     <t>For the estimation of poverty and subsistence incidence, the FIES was utilized for classifying families as poor or non-poor and food poor or non-food poor, respectively, while the LFS was used to classify family members into basic sectors with disaggregation at the national and regional levels. Both FIES and LFS follow the Integrated Survey of Households (ISH) sampling scheme where the sample families in the FIES are generally the same sample families in the LFS.
 The food and poverty thresholds used to identify, whether the families are poor or not, were taken from the Full Year Official Poverty Statistics released by PSA.</t>
+  </si>
+  <si>
+    <t>2023</t>
   </si>
 </sst>
 </file>
@@ -376,7 +379,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -389,9 +392,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -425,9 +425,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -465,7 +465,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -571,7 +571,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -713,7 +713,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -724,7 +724,7 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="N54" sqref="N54"/>
@@ -1838,11 +1838,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5646DEA-C981-45F2-BF15-5300648A4A42}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomRight" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1853,7 +1853,7 @@
     <col min="4" max="10" width="10.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1881,8 +1881,11 @@
       <c r="I1" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1905,7 +1908,7 @@
         <v>10968.529156205745</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1928,7 +1931,7 @@
         <v>21.065909999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1939,7 +1942,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1962,7 +1965,7 @@
         <v>26.339269999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1973,7 +1976,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1996,7 +1999,7 @@
         <v>7638.0556724844619</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -2019,7 +2022,7 @@
         <v>9.1606400000000008</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2030,7 +2033,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2053,7 +2056,7 @@
         <v>12.06002</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -2064,7 +2067,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -2087,7 +2090,7 @@
         <v>28.981400000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -2110,7 +2113,7 @@
         <v>6.1052</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -2133,7 +2136,7 @@
         <v>2.5419800000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -2150,7 +2153,7 @@
         <v>12576.652532652335</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -2167,7 +2170,7 @@
         <v>16.11421</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2178,7 +2181,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -2195,7 +2198,7 @@
         <v>20.999960000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2206,7 +2209,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -2223,7 +2226,7 @@
         <v>8803.8365655750877</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -2240,7 +2243,7 @@
         <v>6.1650900000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -2251,7 +2254,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -2268,7 +2271,7 @@
         <v>8.4680400000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -2279,7 +2282,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -2296,7 +2299,7 @@
         <v>26.949159999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -2313,7 +2316,7 @@
         <v>4.3426499999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -2330,7 +2333,7 @@
         <v>1.7868599999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -2346,8 +2349,11 @@
       <c r="I28" s="1">
         <v>14498.078114544631</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="1">
+        <v>16556.98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -2363,8 +2369,11 @@
       <c r="I29" s="1">
         <v>17.955553145557833</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="1">
+        <v>16.420000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -2380,8 +2389,11 @@
       <c r="I30" s="1">
         <v>4739.8110360999972</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" s="1">
+        <v>4511.8100000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -2397,8 +2409,11 @@
       <c r="I31" s="1">
         <v>23.717926630826302</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" s="1">
+        <v>22.36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -2414,8 +2429,11 @@
       <c r="I32" s="1">
         <v>26136.836813200051</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="1">
+        <v>25241.58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -2431,8 +2449,11 @@
       <c r="I33" s="1">
         <v>10071.257720130052</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="1">
+        <v>11460.21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -2448,8 +2469,11 @@
       <c r="I34" s="1">
         <v>7.0792336675070695</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" s="1">
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -2465,8 +2489,11 @@
       <c r="I35" s="1">
         <v>1868.7383002000088</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" s="1">
+        <v>1616.52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -2482,8 +2509,11 @@
       <c r="I36" s="1">
         <v>9.9320081650149685</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" s="1">
+        <v>8.68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -2499,8 +2529,11 @@
       <c r="I37" s="1">
         <v>10944.939693799992</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" s="1">
+        <v>9794.5499999999993</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -2516,8 +2549,11 @@
       <c r="I38" s="1">
         <v>27.037492166175564</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" s="1">
+        <v>25.62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -2533,8 +2569,11 @@
       <c r="I39" s="1">
         <v>4.8547312751236902</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" s="1">
+        <v>4.21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -2549,6 +2588,9 @@
       </c>
       <c r="I40" s="1">
         <v>1.9483855219994111</v>
+      </c>
+      <c r="J40" s="1">
+        <v>1.63</v>
       </c>
     </row>
   </sheetData>
@@ -2561,8 +2603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37D2146-B4B8-46DC-9C0C-C94E3AE61587}">
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D44" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="J42" sqref="J42"/>
@@ -4207,20 +4249,20 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.5703125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -4228,7 +4270,7 @@
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -4236,19 +4278,19 @@
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="8"/>
+      <c r="B4" s="7"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -4256,7 +4298,7 @@
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>57</v>
       </c>
     </row>
@@ -4264,7 +4306,7 @@
       <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -4272,7 +4314,7 @@
       <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>51</v>
       </c>
     </row>
@@ -4280,7 +4322,7 @@
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>50</v>
       </c>
     </row>
@@ -4288,7 +4330,7 @@
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4296,7 +4338,7 @@
       <c r="A12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>58</v>
       </c>
     </row>
@@ -4304,24 +4346,24 @@
       <c r="A15" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>80</v>
       </c>
     </row>
@@ -4329,100 +4371,103 @@
       <c r="A21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="6" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="6" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="390" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="6" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="6" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="6" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{2EAE60E9-44EE-426E-88DF-14703213F36C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added 2023 Poverty Data
</commit_message>
<xml_diff>
--- a/Data/Poverty/Poverty.xlsx
+++ b/Data/Poverty/Poverty.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Poverty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3261155-FD70-48E6-8484-2EAB479F65D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9BB589-857F-43E2-B3CA-3BED11B92133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E463418E-18EA-45F9-8F1F-BA98B124FBDA}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{E463418E-18EA-45F9-8F1F-BA98B124FBDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Year" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="83">
   <si>
     <t>Indicator</t>
   </si>
@@ -324,6 +324,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -379,7 +382,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -406,6 +409,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -723,11 +727,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23EFC0EE-14C2-43E0-ACDC-93DE3602A4AE}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J39" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N54" sqref="N54"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,7 +742,7 @@
     <col min="4" max="15" width="10.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -781,8 +785,11 @@
       <c r="N1" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -805,7 +812,7 @@
         <v>13823</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -828,7 +835,7 @@
         <v>33.700000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -851,7 +858,7 @@
         <v>5139.5649999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -874,7 +881,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -897,7 +904,7 @@
         <v>30850.191999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -908,7 +915,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -919,7 +926,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -930,7 +937,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -941,7 +948,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -952,7 +959,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -975,7 +982,7 @@
         <v>31.78</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -998,7 +1005,7 @@
         <v>10.71</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1009,7 +1016,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1029,7 +1036,7 @@
         <v>15057.197726169672</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1384,7 +1391,7 @@
         <v>21927.009399999999</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -1407,7 +1414,7 @@
         <v>15189</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -1430,7 +1437,7 @@
         <v>5.7348299999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -1453,7 +1460,7 @@
         <v>1303.549</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -1476,7 +1483,7 @@
         <v>8.0991900000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -1499,7 +1506,7 @@
         <v>8225.7214999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -1522,7 +1529,7 @@
         <v>24.6</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1545,7 +1552,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -1568,7 +1575,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -1587,8 +1594,11 @@
       <c r="N41" s="1">
         <v>28871.319939449077</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41" s="10">
+        <v>33295.99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1</v>
       </c>
@@ -1607,8 +1617,11 @@
       <c r="N42" s="1">
         <v>13.245432215865016</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42" s="10">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -1627,8 +1640,11 @@
       <c r="N43" s="1">
         <v>3496.4584590999966</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43" s="10">
+        <v>2992.01</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -1647,8 +1663,11 @@
       <c r="N44" s="1">
         <v>18.142008108986257</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O44" s="10">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>18</v>
       </c>
@@ -1667,8 +1686,11 @@
       <c r="N45" s="1">
         <v>19992.249267000123</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O45" s="10">
+        <v>17538.86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -1687,8 +1709,11 @@
       <c r="N46" s="1">
         <v>20110.526033729573</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O46" s="10">
+        <v>22994.18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -1707,8 +1732,11 @@
       <c r="N47" s="1">
         <v>3.9374862805873128</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O47" s="10">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -1727,8 +1755,11 @@
       <c r="N48" s="1">
         <v>1039.3966002000031</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O48" s="10">
+        <v>741.73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -1747,8 +1778,11 @@
       <c r="N49" s="1">
         <v>5.9396263055465885</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O49" s="10">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -1767,8 +1801,11 @@
       <c r="N50" s="1">
         <v>6545.3884123500029</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O50" s="10">
+        <v>4837.6400000000003</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -1787,8 +1824,11 @@
       <c r="N51" s="1">
         <v>22.554584635075997</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O51" s="10">
+        <v>20.61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -1807,8 +1847,11 @@
       <c r="N52" s="1">
         <v>2.9874522194088966</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O52" s="10">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -1826,6 +1869,9 @@
       </c>
       <c r="N53" s="1">
         <v>1.0135076257860098</v>
+      </c>
+      <c r="O53" s="10">
+        <v>0.71</v>
       </c>
     </row>
   </sheetData>
@@ -1838,11 +1884,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5646DEA-C981-45F2-BF15-5300648A4A42}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G34" sqref="G34"/>
+      <selection pane="bottomRight" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Monthly inflation update - Aug 2024
</commit_message>
<xml_diff>
--- a/Data/Poverty/Poverty.xlsx
+++ b/Data/Poverty/Poverty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Poverty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74ECD05-FAD3-4B79-ACBF-676B4907D681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C6546D-D311-4D14-88FD-7A488E69C687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E463418E-18EA-45F9-8F1F-BA98B124FBDA}"/>
+    <workbookView xWindow="-1740" yWindow="3270" windowWidth="12810" windowHeight="10545" xr2:uid="{E463418E-18EA-45F9-8F1F-BA98B124FBDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Year" sheetId="1" r:id="rId1"/>
@@ -728,10 +728,10 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomRight" activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1592,7 +1592,7 @@
         <v>25813.497824622897</v>
       </c>
       <c r="N41" s="1">
-        <v>28871.319939449077</v>
+        <v>28794.05</v>
       </c>
       <c r="O41" s="10">
         <v>33295.99</v>
@@ -1615,7 +1615,7 @@
         <v>12.141213642319308</v>
       </c>
       <c r="N42" s="1">
-        <v>13.245432215865016</v>
+        <v>13.2</v>
       </c>
       <c r="O42" s="10">
         <v>10.9</v>
@@ -1638,7 +1638,7 @@
         <v>3004.6072561000165</v>
       </c>
       <c r="N43" s="1">
-        <v>3496.4584590999966</v>
+        <v>3481.83</v>
       </c>
       <c r="O43" s="10">
         <v>2992.01</v>
@@ -1661,7 +1661,7 @@
         <v>16.708595917138165</v>
       </c>
       <c r="N44" s="1">
-        <v>18.142008108986257</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="O44" s="10">
         <v>15.5</v>
@@ -1684,7 +1684,7 @@
         <v>17670.205910017012</v>
       </c>
       <c r="N45" s="1">
-        <v>19992.249267000123</v>
+        <v>19902.75</v>
       </c>
       <c r="O45" s="10">
         <v>17538.86</v>
@@ -1707,7 +1707,7 @@
         <v>18126.108777562113</v>
       </c>
       <c r="N46" s="1">
-        <v>20110.526033729573</v>
+        <v>20046.07</v>
       </c>
       <c r="O46" s="10">
         <v>22994.18</v>
@@ -1730,7 +1730,7 @@
         <v>3.3924762787208991</v>
       </c>
       <c r="N47" s="1">
-        <v>3.9374862805873128</v>
+        <v>3.9</v>
       </c>
       <c r="O47" s="10">
         <v>2.7</v>
@@ -1753,7 +1753,7 @@
         <v>839.54200490000107</v>
       </c>
       <c r="N48" s="1">
-        <v>1039.3966002000031</v>
+        <v>1032.6300000000001</v>
       </c>
       <c r="O48" s="10">
         <v>741.73</v>
@@ -1776,7 +1776,7 @@
         <v>5.2390968558636484</v>
       </c>
       <c r="N49" s="1">
-        <v>5.9396263055465885</v>
+        <v>5.9</v>
       </c>
       <c r="O49" s="10">
         <v>4.3</v>
@@ -1799,7 +1799,7 @@
         <v>5540.6163800201412</v>
       </c>
       <c r="N50" s="1">
-        <v>6545.3884123500029</v>
+        <v>6487.53</v>
       </c>
       <c r="O50" s="10">
         <v>4837.6400000000003</v>
@@ -1822,7 +1822,7 @@
         <v>21.731107023541483</v>
       </c>
       <c r="N51" s="1">
-        <v>22.554584635075997</v>
+        <v>22.52</v>
       </c>
       <c r="O51" s="10">
         <v>20.61</v>
@@ -1845,7 +1845,7 @@
         <v>2.6384201305692279</v>
       </c>
       <c r="N52" s="1">
-        <v>2.9874522194088966</v>
+        <v>2.97</v>
       </c>
       <c r="O52" s="10">
         <v>2.2400000000000002</v>
@@ -1868,7 +1868,7 @@
         <v>0.87039642515473603</v>
       </c>
       <c r="N53" s="1">
-        <v>1.0135076257860098</v>
+        <v>1.01</v>
       </c>
       <c r="O53" s="10">
         <v>0.71</v>

</xml_diff>

<commit_message>
Monthly inflation update - Mar 2025
</commit_message>
<xml_diff>
--- a/Data/Poverty/Poverty.xlsx
+++ b/Data/Poverty/Poverty.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Poverty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C6546D-D311-4D14-88FD-7A488E69C687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF07C85C-2238-4428-A88C-AF9567FBD59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1740" yWindow="3270" windowWidth="12810" windowHeight="10545" xr2:uid="{E463418E-18EA-45F9-8F1F-BA98B124FBDA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E463418E-18EA-45F9-8F1F-BA98B124FBDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Year" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="86">
   <si>
     <t>Indicator</t>
   </si>
@@ -318,6 +318,15 @@
   </si>
   <si>
     <t>2015-2023 (Poverty Statistics)</t>
+  </si>
+  <si>
+    <t>Persons Aged 15 Years and Above with Disability</t>
+  </si>
+  <si>
+    <t>Indigenous Peoples</t>
+  </si>
+  <si>
+    <t>Indigenous Cultural Communities (ICCs) / Indigenous Peoples (IPs) refer to a group of people or homogenous societies identified by self-ascription and ascription by others, who have continuously lived as organized community on communally bounded and defined  territory, and who have, under claims of ownership since time immemorial, occupied, possessed and utilized such territories, sharing common bonds of language, customs, traditions and other distinctive cultural traits, or who have, through resistance  to political, social and cultural inroads of colonization, non-indigenous religions and cultures, became historically differentiated from the majority of Filipinos. The ICCs/IPs shall likewise include peoples who are regarded as indigenous on account of their  descent from the populations which inhabited the country, at the time of conquest or colonization, or at the time of inroads of non-indigenous religions and cultures, or the establishment of present state boundaries, who retain some or all of their  own social, economic, cultural and political institutions, but who may have been displaced from their traditional domains or who may have resettled outside their ancestral domains based on Republic Act No. 8371.</t>
   </si>
 </sst>
 </file>
@@ -727,7 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23EFC0EE-14C2-43E0-ACDC-93DE3602A4AE}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="I38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2647,13 +2656,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37D2146-B4B8-46DC-9C0C-C94E3AE61587}">
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J42" sqref="J42"/>
+      <selection pane="bottomRight" activeCell="J87" sqref="J87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2662,10 +2671,10 @@
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="10" width="10.7109375" style="1" customWidth="1"/>
+    <col min="5" max="11" width="10.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2696,8 +2705,11 @@
       <c r="J1" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -2723,7 +2735,7 @@
         <v>22.499300000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -2737,7 +2749,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -2751,7 +2763,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -2765,7 +2777,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -2791,7 +2803,7 @@
         <v>31.4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -2805,7 +2817,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -2819,7 +2831,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -2833,7 +2845,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -2859,7 +2871,7 @@
         <v>19.381900000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -2873,7 +2885,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -2887,7 +2899,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -2901,7 +2913,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -2927,7 +2939,7 @@
         <v>13.1503</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2941,7 +2953,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -3215,7 +3227,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -3229,7 +3241,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -3255,7 +3267,7 @@
         <v>33.978400000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -3269,7 +3281,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -3283,7 +3295,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -3297,7 +3309,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -3323,7 +3335,7 @@
         <v>25.0136</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -3337,7 +3349,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -3351,7 +3363,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -3365,7 +3377,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -3385,10 +3397,13 @@
         <v>16.558168759736759</v>
       </c>
       <c r="J42" s="1">
-        <v>18.403915621292001</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+        <v>18.3</v>
+      </c>
+      <c r="K42" s="1">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -3408,10 +3423,13 @@
         <v>8655.6983603001045</v>
       </c>
       <c r="J43" s="1">
-        <v>9985.7989651001499</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9940.64</v>
+      </c>
+      <c r="K43" s="1">
+        <v>8662.2000000000007</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>37</v>
       </c>
@@ -3431,10 +3449,13 @@
         <v>5.2173332811708839</v>
       </c>
       <c r="J44" s="1">
-        <v>6.0873192334868804</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="K44" s="1">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -3454,10 +3475,13 @@
         <v>2727.3343919999984</v>
       </c>
       <c r="J45" s="1">
-        <v>3302.9246250000001</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3273.48</v>
+      </c>
+      <c r="K45" s="1">
+        <v>2386</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>35</v>
       </c>
@@ -3477,10 +3501,13 @@
         <v>23.886119310623695</v>
       </c>
       <c r="J46" s="1">
-        <v>26.401041287602698</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+        <v>26.3</v>
+      </c>
+      <c r="K46" s="1">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -3500,10 +3527,13 @@
         <v>9340.7257055000591</v>
       </c>
       <c r="J47" s="1">
-        <v>10463.423518600201</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10425.91</v>
+      </c>
+      <c r="K47" s="1">
+        <v>9294.27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -3523,10 +3553,13 @@
         <v>8.0665061046746622</v>
       </c>
       <c r="J48" s="1">
-        <v>9.4169870468526504</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="K48" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>38</v>
       </c>
@@ -3546,10 +3579,13 @@
         <v>3154.4270521999806</v>
       </c>
       <c r="J49" s="1">
-        <v>3732.1983881999799</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3699.06</v>
+      </c>
+      <c r="K49" s="1">
+        <v>2760.15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>35</v>
       </c>
@@ -3569,10 +3605,13 @@
         <v>14.746623506720944</v>
       </c>
       <c r="J50" s="1">
-        <v>16.581417347140299</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+        <v>16.5</v>
+      </c>
+      <c r="K50" s="1">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -3592,10 +3631,13 @@
         <v>4481.4151366000133</v>
       </c>
       <c r="J51" s="1">
-        <v>5124.1318035000204</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5092.8500000000004</v>
+      </c>
+      <c r="K51" s="1">
+        <v>4386.93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -3615,10 +3657,13 @@
         <v>4.4359836931803081</v>
       </c>
       <c r="J52" s="1">
-        <v>5.1067968737089702</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="K52" s="1">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>38</v>
       </c>
@@ -3638,10 +3683,13 @@
         <v>1348.0702520999978</v>
       </c>
       <c r="J53" s="1">
-        <v>1578.1461697</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1562.63</v>
+      </c>
+      <c r="K53" s="1">
+        <v>1154.51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>35</v>
       </c>
@@ -3661,10 +3709,13 @@
         <v>9.1251097652432041</v>
       </c>
       <c r="J54" s="1">
-        <v>10.259814778598299</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="K54" s="1">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -3684,10 +3735,13 @@
         <v>829.2054251000003</v>
       </c>
       <c r="J55" s="1">
-        <v>1019.2600154</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1015.12</v>
+      </c>
+      <c r="K55" s="1">
+        <v>837.45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>37</v>
       </c>
@@ -3707,10 +3761,13 @@
         <v>2.2269353727442662</v>
       </c>
       <c r="J56" s="1">
-        <v>2.8226748703290498</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.8</v>
+      </c>
+      <c r="K56" s="1">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>38</v>
       </c>
@@ -3730,10 +3787,13 @@
         <v>202.36325260000004</v>
       </c>
       <c r="J57" s="1">
-        <v>280.41828179999999</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+        <v>278.93</v>
+      </c>
+      <c r="K57" s="1">
+        <v>179.67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>35</v>
       </c>
@@ -3753,10 +3813,13 @@
         <v>9.3043550793306657</v>
       </c>
       <c r="J58" s="1">
-        <v>11.6471560559305</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11.6</v>
+      </c>
+      <c r="K58" s="1">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>36</v>
       </c>
@@ -3776,10 +3839,13 @@
         <v>5037.7924518000054</v>
       </c>
       <c r="J59" s="1">
-        <v>6580.9748668000802</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6561.55</v>
+      </c>
+      <c r="K59" s="1">
+        <v>6271.95</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>37</v>
       </c>
@@ -3799,10 +3865,13 @@
         <v>2.6198681930499839</v>
       </c>
       <c r="J60" s="1">
-        <v>3.3166836588497599</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3.3</v>
+      </c>
+      <c r="K60" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>38</v>
       </c>
@@ -3822,10 +3891,13 @@
         <v>1418.5133838000079</v>
       </c>
       <c r="J61" s="1">
-        <v>1874.0207218999999</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1863.34</v>
+      </c>
+      <c r="K61" s="1">
+        <v>1537.71</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>35</v>
       </c>
@@ -3845,10 +3917,13 @@
         <v>24.455686151937428</v>
       </c>
       <c r="J62" s="1">
-        <v>25.6816699304655</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+        <v>25.6</v>
+      </c>
+      <c r="K62" s="1">
+        <v>22.1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>36</v>
       </c>
@@ -3868,10 +3943,13 @@
         <v>12644.425654099812</v>
       </c>
       <c r="J63" s="1">
-        <v>13673.1648926</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+        <v>13603.87</v>
+      </c>
+      <c r="K63" s="1">
+        <v>11352.29</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>37</v>
       </c>
@@ -3891,10 +3969,13 @@
         <v>8.0023639672063833</v>
       </c>
       <c r="J64" s="1">
-        <v>9.0141457279387005</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.9</v>
+      </c>
+      <c r="K64" s="1">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>38</v>
       </c>
@@ -3914,10 +3995,13 @@
         <v>4137.4956978000091</v>
       </c>
       <c r="J65" s="1">
-        <v>4799.2167657999998</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+        <v>4751.47</v>
+      </c>
+      <c r="K65" s="1">
+        <v>3312.85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>35</v>
       </c>
@@ -3937,10 +4021,13 @@
         <v>8.769059525062751</v>
       </c>
       <c r="J66" s="1">
-        <v>10.195046696992399</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="K66" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>36</v>
       </c>
@@ -3960,10 +4047,13 @@
         <v>2385.8834701999958</v>
       </c>
       <c r="J67" s="1">
-        <v>2803.5885965999901</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2797.16</v>
+      </c>
+      <c r="K67" s="1">
+        <v>2502.92</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>37</v>
       </c>
@@ -3983,10 +4073,13 @@
         <v>2.0919469209704937</v>
       </c>
       <c r="J68" s="1">
-        <v>2.6286208974973002</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.6</v>
+      </c>
+      <c r="K68" s="1">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>38</v>
       </c>
@@ -4006,10 +4099,13 @@
         <v>569.17638259999853</v>
       </c>
       <c r="J69" s="1">
-        <v>722.8580498</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+        <v>721.01</v>
+      </c>
+      <c r="K69" s="1">
+        <v>539.11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>35</v>
       </c>
@@ -4029,10 +4125,13 @@
         <v>31.596468444757914</v>
       </c>
       <c r="J70" s="1">
-        <v>30.0161704040068</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+        <v>29.9</v>
+      </c>
+      <c r="K70" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>36</v>
       </c>
@@ -4052,10 +4151,13 @@
         <v>2381.6678780000107</v>
       </c>
       <c r="J71" s="1">
-        <v>2371.4588973</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2359.4</v>
+      </c>
+      <c r="K71" s="1">
+        <v>2102.75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>37</v>
       </c>
@@ -4075,10 +4177,13 @@
         <v>11.484312013255666</v>
       </c>
       <c r="J72" s="1">
-        <v>10.6875658236438</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10.6</v>
+      </c>
+      <c r="K72" s="1">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>38</v>
       </c>
@@ -4098,10 +4203,13 @@
         <v>865.66057440000145</v>
       </c>
       <c r="J73" s="1">
-        <v>844.38230199999805</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+        <v>836.15</v>
+      </c>
+      <c r="K73" s="1">
+        <v>705.48</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>35</v>
       </c>
@@ -4121,10 +4229,13 @@
         <v>26.199814315355429</v>
       </c>
       <c r="J74" s="1">
-        <v>30.636770131799999</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+        <v>30.2</v>
+      </c>
+      <c r="K74" s="1">
+        <v>27.4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>36</v>
       </c>
@@ -4144,10 +4255,13 @@
         <v>287.07144290000036</v>
       </c>
       <c r="J75" s="1">
-        <v>348.2808766</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+        <v>342.76</v>
+      </c>
+      <c r="K75" s="1">
+        <v>353.19</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>37</v>
       </c>
@@ -4167,10 +4281,13 @@
         <v>8.2644355909764045</v>
       </c>
       <c r="J76" s="1">
-        <v>10.772162205654899</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10.5</v>
+      </c>
+      <c r="K76" s="1">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>38</v>
       </c>
@@ -4190,10 +4307,13 @@
         <v>90.553445200000013</v>
       </c>
       <c r="J77" s="1">
-        <v>122.45866909999999</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+        <v>119.66</v>
+      </c>
+      <c r="K77" s="1">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>35</v>
       </c>
@@ -4213,10 +4333,13 @@
         <v>17.986587966677497</v>
       </c>
       <c r="J78" s="1">
-        <v>18.671349623259001</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+        <v>18.5</v>
+      </c>
+      <c r="K78" s="1">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>36</v>
       </c>
@@ -4236,10 +4359,13 @@
         <v>2251.2354339000017</v>
       </c>
       <c r="J79" s="1">
-        <v>2517.8806740999999</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2496.4</v>
+      </c>
+      <c r="K79" s="1">
+        <v>2180.36</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>37</v>
       </c>
@@ -4259,10 +4385,13 @@
         <v>6.245019896879028</v>
       </c>
       <c r="J80" s="1">
-        <v>6.3678341440460402</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6.3</v>
+      </c>
+      <c r="K80" s="1">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>38</v>
       </c>
@@ -4282,7 +4411,170 @@
         <v>781.63852440000051</v>
       </c>
       <c r="J81" s="1">
-        <v>858.71920619999798</v>
+        <v>846.94</v>
+      </c>
+      <c r="K81" s="1">
+        <v>642.38</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>35</v>
+      </c>
+      <c r="B82" t="s">
+        <v>12</v>
+      </c>
+      <c r="C82" t="s">
+        <v>83</v>
+      </c>
+      <c r="D82" t="s">
+        <v>21</v>
+      </c>
+      <c r="I82" s="1">
+        <v>14.7</v>
+      </c>
+      <c r="J82" s="1">
+        <v>17.2</v>
+      </c>
+      <c r="K82" s="1">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>36</v>
+      </c>
+      <c r="B83" t="s">
+        <v>14</v>
+      </c>
+      <c r="C83" t="s">
+        <v>83</v>
+      </c>
+      <c r="D83" t="s">
+        <v>21</v>
+      </c>
+      <c r="I83" s="1">
+        <v>235.94</v>
+      </c>
+      <c r="J83" s="1">
+        <v>270.24</v>
+      </c>
+      <c r="K83" s="1">
+        <v>232.92</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>37</v>
+      </c>
+      <c r="B84" t="s">
+        <v>12</v>
+      </c>
+      <c r="C84" t="s">
+        <v>83</v>
+      </c>
+      <c r="D84" t="s">
+        <v>21</v>
+      </c>
+      <c r="I84" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="J84" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="K84" s="1">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>38</v>
+      </c>
+      <c r="B85" t="s">
+        <v>14</v>
+      </c>
+      <c r="C85" t="s">
+        <v>83</v>
+      </c>
+      <c r="D85" t="s">
+        <v>21</v>
+      </c>
+      <c r="I85" s="1">
+        <v>67.78</v>
+      </c>
+      <c r="J85" s="1">
+        <v>86.02</v>
+      </c>
+      <c r="K85" s="1">
+        <v>59.78</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>35</v>
+      </c>
+      <c r="B86" t="s">
+        <v>12</v>
+      </c>
+      <c r="C86" t="s">
+        <v>84</v>
+      </c>
+      <c r="D86" t="s">
+        <v>21</v>
+      </c>
+      <c r="K86" s="1">
+        <v>32.4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>36</v>
+      </c>
+      <c r="B87" t="s">
+        <v>14</v>
+      </c>
+      <c r="C87" t="s">
+        <v>84</v>
+      </c>
+      <c r="D87" t="s">
+        <v>21</v>
+      </c>
+      <c r="K87" s="1">
+        <v>2925.81</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>37</v>
+      </c>
+      <c r="B88" t="s">
+        <v>12</v>
+      </c>
+      <c r="C88" t="s">
+        <v>84</v>
+      </c>
+      <c r="D88" t="s">
+        <v>21</v>
+      </c>
+      <c r="K88" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>38</v>
+      </c>
+      <c r="B89" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" t="s">
+        <v>84</v>
+      </c>
+      <c r="D89" t="s">
+        <v>21</v>
+      </c>
+      <c r="K89" s="1">
+        <v>1171.47</v>
       </c>
     </row>
   </sheetData>
@@ -4292,10 +4584,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4BEF0A-7E2D-4824-9721-1722416055A8}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4509,6 +4801,14 @@
         <v>74</v>
       </c>
     </row>
+    <row r="33" spans="1:2" ht="405" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{2EAE60E9-44EE-426E-88DF-14703213F36C}"/>

</xml_diff>